<commit_message>
Added data dump for new noise values
</commit_message>
<xml_diff>
--- a/matlab/scripts/optimal_log/Initial_data_analysis.xlsx
+++ b/matlab/scripts/optimal_log/Initial_data_analysis.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MTHE493\Polya_Restoration\matlab\scripts\optimal_log\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cko/repos/school/Polya_Restoration/matlab/scripts/optimal_log/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA504F6D-5016-2C4C-AD6B-DCE5F1E1330D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" xr2:uid="{F5EC45BB-9BF6-4592-8A54-61375F823C90}"/>
+    <workbookView xWindow="80" yWindow="440" windowWidth="28720" windowHeight="17560" xr2:uid="{F5EC45BB-9BF6-4592-8A54-61375F823C90}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="New" sheetId="3" r:id="rId1"/>
+    <sheet name="Old" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">New!$A$1:$I$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Old!$A$1:$I$37</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="62">
   <si>
     <t>Noise Type</t>
   </si>
@@ -93,16 +96,150 @@
   </si>
   <si>
     <t>Speckle + Gauss Markov High</t>
+  </si>
+  <si>
+    <t>aerial1</t>
+  </si>
+  <si>
+    <t>goldengate</t>
+  </si>
+  <si>
+    <t>lena512</t>
+  </si>
+  <si>
+    <t>pentagon</t>
+  </si>
+  <si>
+    <t>N = 50, MSE = 659.0771, PSNR = 19.9414, SSIM = 0.5557</t>
+  </si>
+  <si>
+    <t>N = 2, MSE = 364.7360, PSNR = 22.2222, SSIM = 0.5494</t>
+  </si>
+  <si>
+    <t>N = 50, MSE = 547.1881, PSNR = 20.7494, SSIM = 0.5721</t>
+  </si>
+  <si>
+    <t>N = 2, MSE = 310.1513, PSNR = 22.3713, SSIM = 0.5501</t>
+  </si>
+  <si>
+    <t>N = 2, MSE = 295.6787, PSNR = 22.4797, SSIM = 0.5570</t>
+  </si>
+  <si>
+    <t>N = 2, MSE = 297.4238, PSNR = 22.4685, SSIM = 0.5563</t>
+  </si>
+  <si>
+    <t>N = 4, MSE = 451.8301, PSNR = 21.4685, SSIM = 0.5077</t>
+  </si>
+  <si>
+    <t>N = 2, MSE = 294.5130, PSNR = 22.4844, SSIM = 0.5573</t>
+  </si>
+  <si>
+    <t>N = 2, MSE = 343.2072, PSNR = 22.1382, SSIM = 0.5517</t>
+  </si>
+  <si>
+    <t>N = 50, MSE = 217.5027, PSNR = 24.7562, SSIM = 0.6866</t>
+  </si>
+  <si>
+    <t>N = 4, MSE = 127.6107, PSNR = 27.0719, SSIM = 0.7048</t>
+  </si>
+  <si>
+    <t>N = 37, MSE = 185.9731, PSNR = 25.4363, SSIM = 0.7043</t>
+  </si>
+  <si>
+    <t>N = 4, MSE = 113.9014, PSNR = 27.5655, SSIM = 0.6941</t>
+  </si>
+  <si>
+    <t>N = 3, MSE = 103.6925, PSNR = 27.5503, SSIM = 0.7232</t>
+  </si>
+  <si>
+    <t>N = 3, MSE = 104.7821, PSNR = 27.5253, SSIM = 0.7215</t>
+  </si>
+  <si>
+    <t>N = 8, MSE = 152.2994, PSNR = 26.3038, SSIM = 0.6542</t>
+  </si>
+  <si>
+    <t>N = 3, MSE = 103.0918, PSNR = 27.9986, SSIM = 0.7039</t>
+  </si>
+  <si>
+    <t>N = 5, MSE = 118.7346, PSNR = 27.3850, SSIM = 0.6964</t>
+  </si>
+  <si>
+    <t>N = 47, MSE = 224.6414, PSNR = 24.6159, SSIM = 0.7149</t>
+  </si>
+  <si>
+    <t>N = 6, MSE = 112.6387, PSNR = 27.6139, SSIM = 0.7529</t>
+  </si>
+  <si>
+    <t>N = 27, MSE = 180.3546, PSNR = 25.5695, SSIM = 0.7322</t>
+  </si>
+  <si>
+    <t>N = 5, MSE = 98.4100, PSNR = 28.2004, SSIM = 0.7407</t>
+  </si>
+  <si>
+    <t>N = 4, MSE = 87.9226, PSNR = 28.2707, SSIM = 0.7615</t>
+  </si>
+  <si>
+    <t>N = 5, MSE = 89.1637, PSNR = 28.6289, SSIM = 0.7567</t>
+  </si>
+  <si>
+    <t>N = 8, MSE = 146.8677, PSNR = 26.4615, SSIM = 0.6857</t>
+  </si>
+  <si>
+    <t>N = 5, MSE = 87.2529, PSNR = 28.7230, SSIM = 0.7600</t>
+  </si>
+  <si>
+    <t>N = 6, MSE = 104.5967, PSNR = 27.9356, SSIM = 0.7360</t>
+  </si>
+  <si>
+    <t>N = 50, MSE = 320.6117, PSNR = 23.0710, SSIM = 0.5667</t>
+  </si>
+  <si>
+    <t>N = 4, MSE = 190.1104, PSNR = 25.3407, SSIM = 0.6053</t>
+  </si>
+  <si>
+    <t>N = 45, MSE = 249.5671, PSNR = 24.1589, SSIM = 0.5815</t>
+  </si>
+  <si>
+    <t>N = 4, MSE = 167.9014, PSNR = 25.8803, SSIM = 0.6021</t>
+  </si>
+  <si>
+    <t>N = 3, MSE = 156.2927, PSNR = 26.1914, SSIM = 0.6143</t>
+  </si>
+  <si>
+    <t>N = 3, MSE = 157.5194, PSNR = 26.1575, SSIM = 0.6126</t>
+  </si>
+  <si>
+    <t>N = 8, MSE = 224.6111, PSNR = 24.6165, SSIM = 0.5452</t>
+  </si>
+  <si>
+    <t>N = 3, MSE = 155.7081, PSNR = 26.2077, SSIM = 0.6151</t>
+  </si>
+  <si>
+    <t>N = 4, MSE = 177.9042, PSNR = 25.2950, SSIM = 0.5621</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -134,10 +271,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,21 +590,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33746906-0B72-4A7D-8ACA-AE2BCDFC541B}">
-  <dimension ref="A1:I37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC43DABC-DBC5-8947-9323-9B71ED88D465}">
+  <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L25" sqref="L25"/>
+      <selection pane="topRight" activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -494,11 +633,1219 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
       <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="3">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3">
+        <v>32</v>
+      </c>
+      <c r="E2" s="3">
+        <v>100</v>
+      </c>
+      <c r="F2" s="3">
+        <v>6</v>
+      </c>
+      <c r="G2" s="3">
+        <v>589.524</v>
+      </c>
+      <c r="H2" s="3">
+        <v>20.425999999999998</v>
+      </c>
+      <c r="I2" s="3">
+        <v>0.51300000000000001</v>
+      </c>
+      <c r="K2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="3">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3">
+        <v>256</v>
+      </c>
+      <c r="E3" s="3">
+        <v>100</v>
+      </c>
+      <c r="F3" s="3">
+        <v>3</v>
+      </c>
+      <c r="G3" s="3">
+        <v>314.74200000000002</v>
+      </c>
+      <c r="H3" s="3">
+        <v>23.151</v>
+      </c>
+      <c r="I3" s="3">
+        <v>0.62</v>
+      </c>
+      <c r="K3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="3">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3">
+        <v>128</v>
+      </c>
+      <c r="E4" s="3">
+        <v>100</v>
+      </c>
+      <c r="F4" s="3">
+        <v>2</v>
+      </c>
+      <c r="G4" s="3">
+        <v>500.08499999999998</v>
+      </c>
+      <c r="H4" s="3">
+        <v>21.14</v>
+      </c>
+      <c r="I4" s="3">
+        <v>0.55700000000000005</v>
+      </c>
+      <c r="K4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3">
+        <v>64</v>
+      </c>
+      <c r="E5" s="3">
+        <v>160</v>
+      </c>
+      <c r="F5" s="3">
+        <v>10</v>
+      </c>
+      <c r="G5" s="3">
+        <v>279.11</v>
+      </c>
+      <c r="H5" s="3">
+        <v>23.672999999999998</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0.61799999999999999</v>
+      </c>
+      <c r="K5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3">
+        <v>128</v>
+      </c>
+      <c r="E6" s="3">
+        <v>120</v>
+      </c>
+      <c r="F6" s="3">
+        <v>10</v>
+      </c>
+      <c r="G6" s="3">
+        <v>260.00099999999998</v>
+      </c>
+      <c r="H6" s="3">
+        <v>23.981000000000002</v>
+      </c>
+      <c r="I6" s="3">
+        <v>0.63100000000000001</v>
+      </c>
+      <c r="K6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3">
+        <v>128</v>
+      </c>
+      <c r="E7" s="3">
+        <v>120</v>
+      </c>
+      <c r="F7" s="3">
+        <v>10</v>
+      </c>
+      <c r="G7" s="3">
+        <v>263.75799999999998</v>
+      </c>
+      <c r="H7" s="3">
+        <v>23.919</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0.629</v>
+      </c>
+      <c r="K7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="3">
+        <v>2</v>
+      </c>
+      <c r="D8" s="3">
+        <v>256</v>
+      </c>
+      <c r="E8" s="3">
+        <v>100</v>
+      </c>
+      <c r="F8" s="3">
+        <v>6</v>
+      </c>
+      <c r="G8" s="3">
+        <v>409.666</v>
+      </c>
+      <c r="H8" s="3">
+        <v>22.006</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0.54200000000000004</v>
+      </c>
+      <c r="K8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3">
+        <v>256</v>
+      </c>
+      <c r="E9" s="3">
+        <v>140</v>
+      </c>
+      <c r="F9" s="3">
+        <v>10</v>
+      </c>
+      <c r="G9" s="3">
+        <v>260.74799999999999</v>
+      </c>
+      <c r="H9" s="3">
+        <v>23.969000000000001</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0.63100000000000001</v>
+      </c>
+      <c r="K9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="3">
+        <v>2</v>
+      </c>
+      <c r="D10" s="3">
+        <v>64</v>
+      </c>
+      <c r="E10" s="3">
+        <v>100</v>
+      </c>
+      <c r="F10" s="3">
+        <v>2</v>
+      </c>
+      <c r="G10" s="3">
+        <v>315.17700000000002</v>
+      </c>
+      <c r="H10" s="3">
+        <v>23.145</v>
+      </c>
+      <c r="I10" s="3">
+        <v>0.58899999999999997</v>
+      </c>
+      <c r="K10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="3">
+        <v>3</v>
+      </c>
+      <c r="D11" s="3">
+        <v>64</v>
+      </c>
+      <c r="E11" s="3">
+        <v>100</v>
+      </c>
+      <c r="F11" s="3">
+        <v>6</v>
+      </c>
+      <c r="G11" s="3">
+        <v>182.899</v>
+      </c>
+      <c r="H11" s="3">
+        <v>25.509</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0.70399999999999996</v>
+      </c>
+      <c r="K11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="3">
+        <v>2</v>
+      </c>
+      <c r="D12" s="3">
+        <v>128</v>
+      </c>
+      <c r="E12" s="3">
+        <v>100</v>
+      </c>
+      <c r="F12" s="3">
+        <v>3</v>
+      </c>
+      <c r="G12" s="3">
+        <v>110.94199999999999</v>
+      </c>
+      <c r="H12" s="3">
+        <v>27.68</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0.69299999999999995</v>
+      </c>
+      <c r="K12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="3">
+        <v>3</v>
+      </c>
+      <c r="D13" s="3">
+        <v>64</v>
+      </c>
+      <c r="E13" s="3">
+        <v>100</v>
+      </c>
+      <c r="F13" s="3">
+        <v>7</v>
+      </c>
+      <c r="G13" s="3">
+        <v>157.38399999999999</v>
+      </c>
+      <c r="H13" s="3">
+        <v>26.161000000000001</v>
+      </c>
+      <c r="I13" s="3">
+        <v>0.71599999999999997</v>
+      </c>
+      <c r="K13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="3">
+        <v>2</v>
+      </c>
+      <c r="D14" s="3">
+        <v>128</v>
+      </c>
+      <c r="E14" s="3">
+        <v>100</v>
+      </c>
+      <c r="F14" s="3">
+        <v>4</v>
+      </c>
+      <c r="G14" s="3">
+        <v>107.913</v>
+      </c>
+      <c r="H14" s="3">
+        <v>27.8</v>
+      </c>
+      <c r="I14" s="3">
+        <v>0.69099999999999995</v>
+      </c>
+      <c r="K14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="3">
+        <v>2</v>
+      </c>
+      <c r="D15" s="3">
+        <v>256</v>
+      </c>
+      <c r="E15" s="3">
+        <v>100</v>
+      </c>
+      <c r="F15" s="3">
+        <v>3</v>
+      </c>
+      <c r="G15" s="3">
+        <v>97.566999999999993</v>
+      </c>
+      <c r="H15" s="3">
+        <v>28.238</v>
+      </c>
+      <c r="I15" s="3">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="K15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="3">
+        <v>2</v>
+      </c>
+      <c r="D16" s="3">
+        <v>256</v>
+      </c>
+      <c r="E16" s="3">
+        <v>100</v>
+      </c>
+      <c r="F16" s="3">
+        <v>3</v>
+      </c>
+      <c r="G16" s="3">
+        <v>98.691000000000003</v>
+      </c>
+      <c r="H16" s="3">
+        <v>28.187999999999999</v>
+      </c>
+      <c r="I16" s="3">
+        <v>0.69799999999999995</v>
+      </c>
+      <c r="K16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="3">
+        <v>2</v>
+      </c>
+      <c r="D17" s="3">
+        <v>256</v>
+      </c>
+      <c r="E17" s="3">
+        <v>100</v>
+      </c>
+      <c r="F17" s="3">
+        <v>9</v>
+      </c>
+      <c r="G17" s="3">
+        <v>140.85400000000001</v>
+      </c>
+      <c r="H17" s="3">
+        <v>26.643000000000001</v>
+      </c>
+      <c r="I17" s="3">
+        <v>0.64800000000000002</v>
+      </c>
+      <c r="K17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="3">
+        <v>2</v>
+      </c>
+      <c r="D18" s="3">
+        <v>128</v>
+      </c>
+      <c r="E18" s="3">
+        <v>100</v>
+      </c>
+      <c r="F18" s="3">
+        <v>3</v>
+      </c>
+      <c r="G18" s="3">
+        <v>97.591999999999999</v>
+      </c>
+      <c r="H18" s="3">
+        <v>28.236999999999998</v>
+      </c>
+      <c r="I18" s="3">
+        <v>0.70299999999999996</v>
+      </c>
+      <c r="K18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="3">
+        <v>2</v>
+      </c>
+      <c r="D19" s="3">
+        <v>256</v>
+      </c>
+      <c r="E19" s="3">
+        <v>100</v>
+      </c>
+      <c r="F19" s="3">
+        <v>6</v>
+      </c>
+      <c r="G19" s="3">
+        <v>110.83499999999999</v>
+      </c>
+      <c r="H19" s="3">
+        <v>27.684000000000001</v>
+      </c>
+      <c r="I19" s="3">
+        <v>0.69799999999999995</v>
+      </c>
+      <c r="K19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="3">
+        <v>3</v>
+      </c>
+      <c r="D20" s="3">
+        <v>128</v>
+      </c>
+      <c r="E20" s="3">
+        <v>100</v>
+      </c>
+      <c r="F20" s="3">
+        <v>9</v>
+      </c>
+      <c r="G20" s="3">
+        <v>195.70599999999999</v>
+      </c>
+      <c r="H20" s="3">
+        <v>25.215</v>
+      </c>
+      <c r="I20" s="3">
+        <v>0.746</v>
+      </c>
+      <c r="K20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="3">
+        <v>2</v>
+      </c>
+      <c r="D21" s="3">
+        <v>256</v>
+      </c>
+      <c r="E21" s="3">
+        <v>100</v>
+      </c>
+      <c r="F21" s="3">
+        <v>7</v>
+      </c>
+      <c r="G21" s="3">
+        <v>96.51</v>
+      </c>
+      <c r="H21" s="3">
+        <v>28.285</v>
+      </c>
+      <c r="I21" s="3">
+        <v>0.75700000000000001</v>
+      </c>
+      <c r="K21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="3">
+        <v>3</v>
+      </c>
+      <c r="D22" s="3">
+        <v>256</v>
+      </c>
+      <c r="E22" s="3">
+        <v>100</v>
+      </c>
+      <c r="F22" s="3">
+        <v>8</v>
+      </c>
+      <c r="G22" s="3">
+        <v>155.54599999999999</v>
+      </c>
+      <c r="H22" s="3">
+        <v>26.212</v>
+      </c>
+      <c r="I22" s="3">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="K22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="3">
+        <v>2</v>
+      </c>
+      <c r="D23" s="3">
+        <v>256</v>
+      </c>
+      <c r="E23" s="3">
+        <v>100</v>
+      </c>
+      <c r="F23" s="3">
+        <v>6</v>
+      </c>
+      <c r="G23" s="3">
+        <v>92.981999999999999</v>
+      </c>
+      <c r="H23" s="3">
+        <v>28.446999999999999</v>
+      </c>
+      <c r="I23" s="3">
+        <v>0.74299999999999999</v>
+      </c>
+      <c r="K23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="3">
+        <v>2</v>
+      </c>
+      <c r="D24" s="3">
+        <v>256</v>
+      </c>
+      <c r="E24" s="3">
+        <v>100</v>
+      </c>
+      <c r="F24" s="3">
+        <v>6</v>
+      </c>
+      <c r="G24" s="3">
+        <v>82.798000000000002</v>
+      </c>
+      <c r="H24" s="3">
+        <v>28.951000000000001</v>
+      </c>
+      <c r="I24" s="3">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="K24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="3">
+        <v>2</v>
+      </c>
+      <c r="D25" s="3">
+        <v>256</v>
+      </c>
+      <c r="E25" s="3">
+        <v>100</v>
+      </c>
+      <c r="F25" s="3">
+        <v>6</v>
+      </c>
+      <c r="G25" s="3">
+        <v>83.894000000000005</v>
+      </c>
+      <c r="H25" s="3">
+        <v>28.893000000000001</v>
+      </c>
+      <c r="I25" s="3">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="K25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="3">
+        <v>2</v>
+      </c>
+      <c r="D26" s="3">
+        <v>256</v>
+      </c>
+      <c r="E26" s="3">
+        <v>100</v>
+      </c>
+      <c r="F26" s="3">
+        <v>11</v>
+      </c>
+      <c r="G26" s="3">
+        <v>134.81200000000001</v>
+      </c>
+      <c r="H26" s="3">
+        <v>26.834</v>
+      </c>
+      <c r="I26" s="3">
+        <v>0.68700000000000006</v>
+      </c>
+      <c r="K26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="3">
+        <v>2</v>
+      </c>
+      <c r="D27" s="3">
+        <v>256</v>
+      </c>
+      <c r="E27" s="3">
+        <v>100</v>
+      </c>
+      <c r="F27" s="3">
+        <v>6</v>
+      </c>
+      <c r="G27" s="3">
+        <v>82.085999999999999</v>
+      </c>
+      <c r="H27" s="3">
+        <v>28.988</v>
+      </c>
+      <c r="I27" s="3">
+        <v>0.76300000000000001</v>
+      </c>
+      <c r="K27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="3">
+        <v>2</v>
+      </c>
+      <c r="D28" s="3">
+        <v>128</v>
+      </c>
+      <c r="E28" s="3">
+        <v>100</v>
+      </c>
+      <c r="F28" s="3">
+        <v>7</v>
+      </c>
+      <c r="G28" s="3">
+        <v>97.521000000000001</v>
+      </c>
+      <c r="H28" s="3">
+        <v>28.24</v>
+      </c>
+      <c r="I28" s="3">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="K28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" s="3">
+        <v>3</v>
+      </c>
+      <c r="D29" s="3">
+        <v>256</v>
+      </c>
+      <c r="E29" s="3">
+        <v>100</v>
+      </c>
+      <c r="F29" s="3">
+        <v>12</v>
+      </c>
+      <c r="G29" s="3">
+        <v>292.71300000000002</v>
+      </c>
+      <c r="H29" s="3">
+        <v>23.466000000000001</v>
+      </c>
+      <c r="I29" s="3">
+        <v>0.55200000000000005</v>
+      </c>
+      <c r="K29" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="3">
+        <v>3</v>
+      </c>
+      <c r="D30" s="3">
+        <v>256</v>
+      </c>
+      <c r="E30" s="3">
+        <v>100</v>
+      </c>
+      <c r="F30" s="3">
+        <v>2</v>
+      </c>
+      <c r="G30" s="3">
+        <v>184.626</v>
+      </c>
+      <c r="H30" s="3">
+        <v>25.468</v>
+      </c>
+      <c r="I30" s="3">
+        <v>0.58699999999999997</v>
+      </c>
+      <c r="K30" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" s="3">
+        <v>3</v>
+      </c>
+      <c r="D31" s="3">
+        <v>64</v>
+      </c>
+      <c r="E31" s="3">
+        <v>100</v>
+      </c>
+      <c r="F31" s="3">
+        <v>7</v>
+      </c>
+      <c r="G31" s="3">
+        <v>247.785</v>
+      </c>
+      <c r="H31" s="3">
+        <v>24.19</v>
+      </c>
+      <c r="I31" s="3">
+        <v>0.55900000000000005</v>
+      </c>
+      <c r="K31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>21</v>
+      </c>
+      <c r="B32" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="3">
+        <v>2</v>
+      </c>
+      <c r="D32" s="3">
+        <v>256</v>
+      </c>
+      <c r="E32" s="3">
+        <v>100</v>
+      </c>
+      <c r="F32" s="3">
+        <v>3</v>
+      </c>
+      <c r="G32" s="3">
+        <v>165.821</v>
+      </c>
+      <c r="H32" s="3">
+        <v>25.934000000000001</v>
+      </c>
+      <c r="I32" s="3">
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="K32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" s="3">
+        <v>2</v>
+      </c>
+      <c r="D33" s="3">
+        <v>256</v>
+      </c>
+      <c r="E33" s="3">
+        <v>100</v>
+      </c>
+      <c r="F33" s="3">
+        <v>3</v>
+      </c>
+      <c r="G33" s="3">
+        <v>154.28</v>
+      </c>
+      <c r="H33" s="3">
+        <v>26.248000000000001</v>
+      </c>
+      <c r="I33" s="3">
+        <v>0.61</v>
+      </c>
+      <c r="K33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" s="3">
+        <v>2</v>
+      </c>
+      <c r="D34" s="3">
+        <v>256</v>
+      </c>
+      <c r="E34" s="3">
+        <v>100</v>
+      </c>
+      <c r="F34" s="3">
+        <v>3</v>
+      </c>
+      <c r="G34" s="3">
+        <v>155.50200000000001</v>
+      </c>
+      <c r="H34" s="3">
+        <v>26.213000000000001</v>
+      </c>
+      <c r="I34" s="3">
+        <v>0.60799999999999998</v>
+      </c>
+      <c r="K34" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35" s="3">
+        <v>2</v>
+      </c>
+      <c r="D35" s="3">
+        <v>256</v>
+      </c>
+      <c r="E35" s="3">
+        <v>100</v>
+      </c>
+      <c r="F35" s="3">
+        <v>11</v>
+      </c>
+      <c r="G35" s="3">
+        <v>215.56700000000001</v>
+      </c>
+      <c r="H35" s="3">
+        <v>24.795000000000002</v>
+      </c>
+      <c r="I35" s="3">
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="K35" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>13</v>
+      </c>
+      <c r="B36" t="s">
+        <v>25</v>
+      </c>
+      <c r="C36" s="3">
+        <v>2</v>
+      </c>
+      <c r="D36" s="3">
+        <v>256</v>
+      </c>
+      <c r="E36" s="3">
+        <v>100</v>
+      </c>
+      <c r="F36" s="3">
+        <v>3</v>
+      </c>
+      <c r="G36" s="3">
+        <v>153.62100000000001</v>
+      </c>
+      <c r="H36" s="3">
+        <v>26.265999999999998</v>
+      </c>
+      <c r="I36" s="3">
+        <v>0.61099999999999999</v>
+      </c>
+      <c r="K36" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" t="s">
+        <v>25</v>
+      </c>
+      <c r="C37" s="3">
+        <v>2</v>
+      </c>
+      <c r="D37" s="3">
+        <v>256</v>
+      </c>
+      <c r="E37" s="3">
+        <v>100</v>
+      </c>
+      <c r="F37" s="3">
+        <v>6</v>
+      </c>
+      <c r="G37" s="3">
+        <v>173.547</v>
+      </c>
+      <c r="H37" s="3">
+        <v>25.736999999999998</v>
+      </c>
+      <c r="I37" s="3">
+        <v>0.59</v>
+      </c>
+      <c r="K37" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:I37" xr:uid="{EA99F5D4-17E7-4E3A-AD12-CAED7081E540}">
+    <sortState ref="A2:B37">
+      <sortCondition ref="A20"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33746906-0B72-4A7D-8ACA-AE2BCDFC541B}">
+  <dimension ref="A1:I37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection activeCell="A8" sqref="A8"/>
+      <selection pane="topRight" activeCell="A35" sqref="A35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="1">
@@ -523,7 +1870,7 @@
         <v>0.31900000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -552,7 +1899,7 @@
         <v>0.48299999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -581,7 +1928,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -610,7 +1957,7 @@
         <v>0.373</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -639,7 +1986,7 @@
         <v>0.57299999999999995</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -668,7 +2015,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -697,7 +2044,7 @@
         <v>0.70899999999999996</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -726,7 +2073,7 @@
         <v>0.55700000000000005</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -755,7 +2102,7 @@
         <v>0.49299999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -784,7 +2131,7 @@
         <v>0.68300000000000005</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -813,7 +2160,7 @@
         <v>0.71899999999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -842,7 +2189,7 @@
         <v>0.52800000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -871,7 +2218,7 @@
         <v>0.41899999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -900,7 +2247,7 @@
         <v>0.49299999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -929,7 +2276,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -958,7 +2305,7 @@
         <v>0.42499999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -987,7 +2334,7 @@
         <v>0.56799999999999995</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1016,7 +2363,7 @@
         <v>0.63500000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1045,7 +2392,7 @@
         <v>0.72499999999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1074,7 +2421,7 @@
         <v>0.54800000000000004</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1103,7 +2450,7 @@
         <v>0.51400000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -1132,7 +2479,7 @@
         <v>0.60599999999999998</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -1161,7 +2508,7 @@
         <v>0.65700000000000003</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -1190,7 +2537,7 @@
         <v>0.496</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -1219,7 +2566,7 @@
         <v>0.42899999999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -1248,7 +2595,7 @@
         <v>0.626</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>15</v>
       </c>
@@ -1277,7 +2624,7 @@
         <v>0.65200000000000002</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>15</v>
       </c>
@@ -1306,7 +2653,7 @@
         <v>0.48099999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>13</v>
       </c>
@@ -1335,7 +2682,7 @@
         <v>0.58199999999999996</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>13</v>
       </c>
@@ -1364,7 +2711,7 @@
         <v>0.68100000000000005</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>13</v>
       </c>
@@ -1393,7 +2740,7 @@
         <v>0.72199999999999998</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>13</v>
       </c>
@@ -1422,7 +2769,7 @@
         <v>0.57599999999999996</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>14</v>
       </c>
@@ -1451,7 +2798,7 @@
         <v>0.48599999999999999</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>14</v>
       </c>
@@ -1480,7 +2827,7 @@
         <v>0.66500000000000004</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -1509,7 +2856,7 @@
         <v>0.69399999999999995</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
Formatted median data dump
</commit_message>
<xml_diff>
--- a/matlab/scripts/optimal_log/Initial_data_analysis.xlsx
+++ b/matlab/scripts/optimal_log/Initial_data_analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cko/repos/school/Polya_Restoration/matlab/scripts/optimal_log/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA504F6D-5016-2C4C-AD6B-DCE5F1E1330D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CB7A42F-DB8B-7B49-BC27-B745A8E1D12C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="440" windowWidth="28720" windowHeight="17560" xr2:uid="{F5EC45BB-9BF6-4592-8A54-61375F823C90}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Old" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">New!$A$1:$I$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">New!$A$1:$M$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Old!$A$1:$I$37</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="27">
   <si>
     <t>Noise Type</t>
   </si>
@@ -110,112 +110,7 @@
     <t>pentagon</t>
   </si>
   <si>
-    <t>N = 50, MSE = 659.0771, PSNR = 19.9414, SSIM = 0.5557</t>
-  </si>
-  <si>
-    <t>N = 2, MSE = 364.7360, PSNR = 22.2222, SSIM = 0.5494</t>
-  </si>
-  <si>
-    <t>N = 50, MSE = 547.1881, PSNR = 20.7494, SSIM = 0.5721</t>
-  </si>
-  <si>
-    <t>N = 2, MSE = 310.1513, PSNR = 22.3713, SSIM = 0.5501</t>
-  </si>
-  <si>
-    <t>N = 2, MSE = 295.6787, PSNR = 22.4797, SSIM = 0.5570</t>
-  </si>
-  <si>
-    <t>N = 2, MSE = 297.4238, PSNR = 22.4685, SSIM = 0.5563</t>
-  </si>
-  <si>
-    <t>N = 4, MSE = 451.8301, PSNR = 21.4685, SSIM = 0.5077</t>
-  </si>
-  <si>
-    <t>N = 2, MSE = 294.5130, PSNR = 22.4844, SSIM = 0.5573</t>
-  </si>
-  <si>
-    <t>N = 2, MSE = 343.2072, PSNR = 22.1382, SSIM = 0.5517</t>
-  </si>
-  <si>
-    <t>N = 50, MSE = 217.5027, PSNR = 24.7562, SSIM = 0.6866</t>
-  </si>
-  <si>
-    <t>N = 4, MSE = 127.6107, PSNR = 27.0719, SSIM = 0.7048</t>
-  </si>
-  <si>
-    <t>N = 37, MSE = 185.9731, PSNR = 25.4363, SSIM = 0.7043</t>
-  </si>
-  <si>
-    <t>N = 4, MSE = 113.9014, PSNR = 27.5655, SSIM = 0.6941</t>
-  </si>
-  <si>
-    <t>N = 3, MSE = 103.6925, PSNR = 27.5503, SSIM = 0.7232</t>
-  </si>
-  <si>
-    <t>N = 3, MSE = 104.7821, PSNR = 27.5253, SSIM = 0.7215</t>
-  </si>
-  <si>
-    <t>N = 8, MSE = 152.2994, PSNR = 26.3038, SSIM = 0.6542</t>
-  </si>
-  <si>
-    <t>N = 3, MSE = 103.0918, PSNR = 27.9986, SSIM = 0.7039</t>
-  </si>
-  <si>
-    <t>N = 5, MSE = 118.7346, PSNR = 27.3850, SSIM = 0.6964</t>
-  </si>
-  <si>
-    <t>N = 47, MSE = 224.6414, PSNR = 24.6159, SSIM = 0.7149</t>
-  </si>
-  <si>
-    <t>N = 6, MSE = 112.6387, PSNR = 27.6139, SSIM = 0.7529</t>
-  </si>
-  <si>
-    <t>N = 27, MSE = 180.3546, PSNR = 25.5695, SSIM = 0.7322</t>
-  </si>
-  <si>
-    <t>N = 5, MSE = 98.4100, PSNR = 28.2004, SSIM = 0.7407</t>
-  </si>
-  <si>
-    <t>N = 4, MSE = 87.9226, PSNR = 28.2707, SSIM = 0.7615</t>
-  </si>
-  <si>
-    <t>N = 5, MSE = 89.1637, PSNR = 28.6289, SSIM = 0.7567</t>
-  </si>
-  <si>
-    <t>N = 8, MSE = 146.8677, PSNR = 26.4615, SSIM = 0.6857</t>
-  </si>
-  <si>
-    <t>N = 5, MSE = 87.2529, PSNR = 28.7230, SSIM = 0.7600</t>
-  </si>
-  <si>
-    <t>N = 6, MSE = 104.5967, PSNR = 27.9356, SSIM = 0.7360</t>
-  </si>
-  <si>
-    <t>N = 50, MSE = 320.6117, PSNR = 23.0710, SSIM = 0.5667</t>
-  </si>
-  <si>
-    <t>N = 4, MSE = 190.1104, PSNR = 25.3407, SSIM = 0.6053</t>
-  </si>
-  <si>
-    <t>N = 45, MSE = 249.5671, PSNR = 24.1589, SSIM = 0.5815</t>
-  </si>
-  <si>
-    <t>N = 4, MSE = 167.9014, PSNR = 25.8803, SSIM = 0.6021</t>
-  </si>
-  <si>
-    <t>N = 3, MSE = 156.2927, PSNR = 26.1914, SSIM = 0.6143</t>
-  </si>
-  <si>
-    <t>N = 3, MSE = 157.5194, PSNR = 26.1575, SSIM = 0.6126</t>
-  </si>
-  <si>
-    <t>N = 8, MSE = 224.6111, PSNR = 24.6165, SSIM = 0.5452</t>
-  </si>
-  <si>
-    <t>N = 3, MSE = 155.7081, PSNR = 26.2077, SSIM = 0.6151</t>
-  </si>
-  <si>
-    <t>N = 4, MSE = 177.9042, PSNR = 25.2950, SSIM = 0.5621</t>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -591,11 +486,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC43DABC-DBC5-8947-9323-9B71ED88D465}">
-  <dimension ref="A1:K37"/>
+  <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K37" sqref="K37"/>
+      <selection pane="topRight" activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -604,7 +499,7 @@
     <col min="2" max="2" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -632,8 +527,20 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -661,11 +568,20 @@
       <c r="I2" s="3">
         <v>0.51300000000000001</v>
       </c>
-      <c r="K2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="J2">
+        <v>50</v>
+      </c>
+      <c r="K2">
+        <v>659.07709999999997</v>
+      </c>
+      <c r="L2">
+        <v>19.941400000000002</v>
+      </c>
+      <c r="M2">
+        <v>0.55569999999999997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -693,11 +609,20 @@
       <c r="I3" s="3">
         <v>0.62</v>
       </c>
-      <c r="K3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>364.73599999999999</v>
+      </c>
+      <c r="L3">
+        <v>22.222200000000001</v>
+      </c>
+      <c r="M3">
+        <v>0.5494</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -725,11 +650,20 @@
       <c r="I4" s="3">
         <v>0.55700000000000005</v>
       </c>
-      <c r="K4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="J4">
+        <v>50</v>
+      </c>
+      <c r="K4">
+        <v>547.18809999999996</v>
+      </c>
+      <c r="L4">
+        <v>20.749400000000001</v>
+      </c>
+      <c r="M4">
+        <v>0.57210000000000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -757,11 +691,20 @@
       <c r="I5" s="3">
         <v>0.61799999999999999</v>
       </c>
-      <c r="K5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="J5">
+        <v>2</v>
+      </c>
+      <c r="K5">
+        <v>310.15129999999999</v>
+      </c>
+      <c r="L5">
+        <v>22.371300000000002</v>
+      </c>
+      <c r="M5">
+        <v>0.55010000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>19</v>
       </c>
@@ -789,11 +732,20 @@
       <c r="I6" s="3">
         <v>0.63100000000000001</v>
       </c>
-      <c r="K6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="J6">
+        <v>2</v>
+      </c>
+      <c r="K6">
+        <v>295.67869999999999</v>
+      </c>
+      <c r="L6">
+        <v>22.479700000000001</v>
+      </c>
+      <c r="M6">
+        <v>0.55700000000000005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -821,11 +773,20 @@
       <c r="I7" s="3">
         <v>0.629</v>
       </c>
-      <c r="K7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="J7">
+        <v>2</v>
+      </c>
+      <c r="K7">
+        <v>297.42380000000003</v>
+      </c>
+      <c r="L7">
+        <v>22.468499999999999</v>
+      </c>
+      <c r="M7">
+        <v>0.55630000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -853,11 +814,20 @@
       <c r="I8" s="3">
         <v>0.54200000000000004</v>
       </c>
-      <c r="K8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="J8">
+        <v>4</v>
+      </c>
+      <c r="K8">
+        <v>451.83010000000002</v>
+      </c>
+      <c r="L8">
+        <v>21.468499999999999</v>
+      </c>
+      <c r="M8">
+        <v>0.50770000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -885,11 +855,20 @@
       <c r="I9" s="3">
         <v>0.63100000000000001</v>
       </c>
-      <c r="K9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="J9">
+        <v>2</v>
+      </c>
+      <c r="K9">
+        <v>294.51299999999998</v>
+      </c>
+      <c r="L9">
+        <v>22.484400000000001</v>
+      </c>
+      <c r="M9">
+        <v>0.55730000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -917,11 +896,20 @@
       <c r="I10" s="3">
         <v>0.58899999999999997</v>
       </c>
-      <c r="K10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="J10">
+        <v>2</v>
+      </c>
+      <c r="K10">
+        <v>343.2072</v>
+      </c>
+      <c r="L10">
+        <v>22.138200000000001</v>
+      </c>
+      <c r="M10">
+        <v>0.55169999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -949,11 +937,20 @@
       <c r="I11" s="3">
         <v>0.70399999999999996</v>
       </c>
-      <c r="K11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="J11">
+        <v>50</v>
+      </c>
+      <c r="K11">
+        <v>217.5027</v>
+      </c>
+      <c r="L11">
+        <v>24.7562</v>
+      </c>
+      <c r="M11">
+        <v>0.68659999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -981,11 +978,20 @@
       <c r="I12" s="3">
         <v>0.69299999999999995</v>
       </c>
-      <c r="K12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="J12">
+        <v>4</v>
+      </c>
+      <c r="K12">
+        <v>127.61069999999999</v>
+      </c>
+      <c r="L12">
+        <v>27.071899999999999</v>
+      </c>
+      <c r="M12">
+        <v>0.70479999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1013,11 +1019,20 @@
       <c r="I13" s="3">
         <v>0.71599999999999997</v>
       </c>
-      <c r="K13" t="s">
+      <c r="J13">
         <v>37</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="K13">
+        <v>185.97309999999999</v>
+      </c>
+      <c r="L13">
+        <v>25.436299999999999</v>
+      </c>
+      <c r="M13">
+        <v>0.70430000000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1045,11 +1060,20 @@
       <c r="I14" s="3">
         <v>0.69099999999999995</v>
       </c>
-      <c r="K14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="J14">
+        <v>4</v>
+      </c>
+      <c r="K14">
+        <v>113.9014</v>
+      </c>
+      <c r="L14">
+        <v>27.5655</v>
+      </c>
+      <c r="M14">
+        <v>0.69410000000000005</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>19</v>
       </c>
@@ -1077,11 +1101,20 @@
       <c r="I15" s="3">
         <v>0.70199999999999996</v>
       </c>
-      <c r="K15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="J15">
+        <v>3</v>
+      </c>
+      <c r="K15">
+        <v>103.6925</v>
+      </c>
+      <c r="L15">
+        <v>27.5503</v>
+      </c>
+      <c r="M15">
+        <v>0.72319999999999995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1109,11 +1142,20 @@
       <c r="I16" s="3">
         <v>0.69799999999999995</v>
       </c>
-      <c r="K16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="J16">
+        <v>3</v>
+      </c>
+      <c r="K16">
+        <v>104.7821</v>
+      </c>
+      <c r="L16">
+        <v>27.525300000000001</v>
+      </c>
+      <c r="M16">
+        <v>0.72150000000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1141,11 +1183,20 @@
       <c r="I17" s="3">
         <v>0.64800000000000002</v>
       </c>
-      <c r="K17" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="J17">
+        <v>8</v>
+      </c>
+      <c r="K17">
+        <v>152.29939999999999</v>
+      </c>
+      <c r="L17">
+        <v>26.303799999999999</v>
+      </c>
+      <c r="M17">
+        <v>0.6542</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -1173,11 +1224,20 @@
       <c r="I18" s="3">
         <v>0.70299999999999996</v>
       </c>
-      <c r="K18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="J18">
+        <v>3</v>
+      </c>
+      <c r="K18">
+        <v>103.09180000000001</v>
+      </c>
+      <c r="L18">
+        <v>27.9986</v>
+      </c>
+      <c r="M18">
+        <v>0.70389999999999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -1205,11 +1265,20 @@
       <c r="I19" s="3">
         <v>0.69799999999999995</v>
       </c>
-      <c r="K19" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="J19">
+        <v>5</v>
+      </c>
+      <c r="K19">
+        <v>118.7346</v>
+      </c>
+      <c r="L19">
+        <v>27.385000000000002</v>
+      </c>
+      <c r="M19">
+        <v>0.69640000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1237,11 +1306,20 @@
       <c r="I20" s="3">
         <v>0.746</v>
       </c>
-      <c r="K20" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="J20">
+        <v>47</v>
+      </c>
+      <c r="K20">
+        <v>224.6414</v>
+      </c>
+      <c r="L20">
+        <v>24.6159</v>
+      </c>
+      <c r="M20">
+        <v>0.71489999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -1269,11 +1347,20 @@
       <c r="I21" s="3">
         <v>0.75700000000000001</v>
       </c>
-      <c r="K21" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="J21">
+        <v>6</v>
+      </c>
+      <c r="K21">
+        <v>112.6387</v>
+      </c>
+      <c r="L21">
+        <v>27.613900000000001</v>
+      </c>
+      <c r="M21">
+        <v>0.75290000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -1301,11 +1388,20 @@
       <c r="I22" s="3">
         <v>0.75900000000000001</v>
       </c>
-      <c r="K22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="J22">
+        <v>27</v>
+      </c>
+      <c r="K22">
+        <v>180.3546</v>
+      </c>
+      <c r="L22">
+        <v>25.569500000000001</v>
+      </c>
+      <c r="M22">
+        <v>0.73219999999999996</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1333,11 +1429,20 @@
       <c r="I23" s="3">
         <v>0.74299999999999999</v>
       </c>
-      <c r="K23" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="J23">
+        <v>5</v>
+      </c>
+      <c r="K23">
+        <v>98.41</v>
+      </c>
+      <c r="L23">
+        <v>28.200399999999998</v>
+      </c>
+      <c r="M23">
+        <v>0.74070000000000003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>19</v>
       </c>
@@ -1365,11 +1470,20 @@
       <c r="I24" s="3">
         <v>0.76100000000000001</v>
       </c>
-      <c r="K24" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="J24">
+        <v>4</v>
+      </c>
+      <c r="K24">
+        <v>87.922600000000003</v>
+      </c>
+      <c r="L24">
+        <v>28.270700000000001</v>
+      </c>
+      <c r="M24">
+        <v>0.76149999999999995</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -1397,11 +1511,20 @@
       <c r="I25" s="3">
         <v>0.75900000000000001</v>
       </c>
-      <c r="K25" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="J25">
+        <v>5</v>
+      </c>
+      <c r="K25">
+        <v>89.163700000000006</v>
+      </c>
+      <c r="L25">
+        <v>28.628900000000002</v>
+      </c>
+      <c r="M25">
+        <v>0.75670000000000004</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -1429,11 +1552,20 @@
       <c r="I26" s="3">
         <v>0.68700000000000006</v>
       </c>
-      <c r="K26" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="J26">
+        <v>8</v>
+      </c>
+      <c r="K26">
+        <v>146.86770000000001</v>
+      </c>
+      <c r="L26">
+        <v>26.461500000000001</v>
+      </c>
+      <c r="M26">
+        <v>0.68569999999999998</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>13</v>
       </c>
@@ -1461,11 +1593,20 @@
       <c r="I27" s="3">
         <v>0.76300000000000001</v>
       </c>
-      <c r="K27" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="J27">
+        <v>5</v>
+      </c>
+      <c r="K27">
+        <v>87.252899999999997</v>
+      </c>
+      <c r="L27">
+        <v>28.722999999999999</v>
+      </c>
+      <c r="M27">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -1493,11 +1634,20 @@
       <c r="I28" s="3">
         <v>0.73499999999999999</v>
       </c>
-      <c r="K28" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="J28">
+        <v>6</v>
+      </c>
+      <c r="K28">
+        <v>104.5967</v>
+      </c>
+      <c r="L28">
+        <v>27.935600000000001</v>
+      </c>
+      <c r="M28">
+        <v>0.73599999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -1525,11 +1675,20 @@
       <c r="I29" s="3">
         <v>0.55200000000000005</v>
       </c>
-      <c r="K29" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="J29">
+        <v>50</v>
+      </c>
+      <c r="K29">
+        <v>320.61169999999998</v>
+      </c>
+      <c r="L29">
+        <v>23.071000000000002</v>
+      </c>
+      <c r="M29">
+        <v>0.56669999999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>16</v>
       </c>
@@ -1557,11 +1716,20 @@
       <c r="I30" s="3">
         <v>0.58699999999999997</v>
       </c>
-      <c r="K30" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="J30">
+        <v>4</v>
+      </c>
+      <c r="K30">
+        <v>190.1104</v>
+      </c>
+      <c r="L30">
+        <v>25.340699999999998</v>
+      </c>
+      <c r="M30">
+        <v>0.60529999999999995</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>17</v>
       </c>
@@ -1589,11 +1757,20 @@
       <c r="I31" s="3">
         <v>0.55900000000000005</v>
       </c>
-      <c r="K31" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="J31">
+        <v>45</v>
+      </c>
+      <c r="K31">
+        <v>249.56710000000001</v>
+      </c>
+      <c r="L31">
+        <v>24.158899999999999</v>
+      </c>
+      <c r="M31">
+        <v>0.58150000000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>21</v>
       </c>
@@ -1621,11 +1798,20 @@
       <c r="I32" s="3">
         <v>0.59499999999999997</v>
       </c>
-      <c r="K32" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="J32">
+        <v>4</v>
+      </c>
+      <c r="K32">
+        <v>167.9014</v>
+      </c>
+      <c r="L32">
+        <v>25.880299999999998</v>
+      </c>
+      <c r="M32">
+        <v>0.60209999999999997</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>19</v>
       </c>
@@ -1653,11 +1839,20 @@
       <c r="I33" s="3">
         <v>0.61</v>
       </c>
-      <c r="K33" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="J33">
+        <v>3</v>
+      </c>
+      <c r="K33">
+        <v>156.2927</v>
+      </c>
+      <c r="L33">
+        <v>26.191400000000002</v>
+      </c>
+      <c r="M33">
+        <v>0.61429999999999996</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>20</v>
       </c>
@@ -1685,11 +1880,20 @@
       <c r="I34" s="3">
         <v>0.60799999999999998</v>
       </c>
-      <c r="K34" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="J34">
+        <v>3</v>
+      </c>
+      <c r="K34">
+        <v>157.51939999999999</v>
+      </c>
+      <c r="L34">
+        <v>26.157499999999999</v>
+      </c>
+      <c r="M34">
+        <v>0.61260000000000003</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>15</v>
       </c>
@@ -1717,11 +1921,20 @@
       <c r="I35" s="3">
         <v>0.54500000000000004</v>
       </c>
-      <c r="K35" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="J35">
+        <v>8</v>
+      </c>
+      <c r="K35">
+        <v>224.61109999999999</v>
+      </c>
+      <c r="L35">
+        <v>24.616499999999998</v>
+      </c>
+      <c r="M35">
+        <v>0.54520000000000002</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>13</v>
       </c>
@@ -1749,11 +1962,20 @@
       <c r="I36" s="3">
         <v>0.61099999999999999</v>
       </c>
-      <c r="K36" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="J36">
+        <v>3</v>
+      </c>
+      <c r="K36">
+        <v>155.7081</v>
+      </c>
+      <c r="L36">
+        <v>26.207699999999999</v>
+      </c>
+      <c r="M36">
+        <v>0.61509999999999998</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>14</v>
       </c>
@@ -1781,16 +2003,21 @@
       <c r="I37" s="3">
         <v>0.59</v>
       </c>
-      <c r="K37" t="s">
-        <v>61</v>
+      <c r="J37">
+        <v>4</v>
+      </c>
+      <c r="K37">
+        <v>177.9042</v>
+      </c>
+      <c r="L37">
+        <v>25.295000000000002</v>
+      </c>
+      <c r="M37">
+        <v>0.56210000000000004</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I37" xr:uid="{EA99F5D4-17E7-4E3A-AD12-CAED7081E540}">
-    <sortState ref="A2:B37">
-      <sortCondition ref="A20"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:M1" xr:uid="{E1048CE1-163E-9243-951A-AD61112252EC}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed Edge Map column.
</commit_message>
<xml_diff>
--- a/matlab/scripts/optimal_log/Initial_data_analysis.xlsx
+++ b/matlab/scripts/optimal_log/Initial_data_analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MTHE493\Polya_Restoration\matlab\scripts\optimal_log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C82FE5B-3627-4440-8B2A-45799F0147F7}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2422A8CD-EFD4-43D7-A691-DA1983453A51}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="444" windowWidth="28716" windowHeight="17556" xr2:uid="{F5EC45BB-9BF6-4592-8A54-61375F823C90}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Old" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">New!$A$1:$V$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">New!$A$1:$V$73</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Old!$A$1:$I$37</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
@@ -551,9 +551,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC43DABC-DBC5-8947-9323-9B71ED88D465}">
   <dimension ref="A1:V73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="W8" sqref="W8"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C38" sqref="C38:C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -654,7 +654,7 @@
         <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D2">
         <v>3838.1801</v>
@@ -724,7 +724,7 @@
         <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D3">
         <v>1414.6353999999999</v>
@@ -794,7 +794,7 @@
         <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D4">
         <v>2783.5153</v>
@@ -864,7 +864,7 @@
         <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D5">
         <v>823.60310000000004</v>
@@ -934,7 +934,7 @@
         <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D6">
         <v>787.52650000000006</v>
@@ -1004,7 +1004,7 @@
         <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D7">
         <v>790.45280000000002</v>
@@ -1074,7 +1074,7 @@
         <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D8">
         <v>1651.6928</v>
@@ -1144,7 +1144,7 @@
         <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D9">
         <v>788.12850000000003</v>
@@ -1214,7 +1214,7 @@
         <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D10">
         <v>1038.6316999999999</v>
@@ -1284,7 +1284,7 @@
         <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D11">
         <v>1667.9771000000001</v>
@@ -1354,7 +1354,7 @@
         <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D12">
         <v>661.21640000000002</v>
@@ -1424,7 +1424,7 @@
         <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D13">
         <v>1249.7942</v>
@@ -1494,7 +1494,7 @@
         <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D14">
         <v>454.9683</v>
@@ -1564,7 +1564,7 @@
         <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D15">
         <v>402.68029999999999</v>
@@ -1634,7 +1634,7 @@
         <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D16">
         <v>408.50029999999998</v>
@@ -1704,7 +1704,7 @@
         <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D17">
         <v>963.07600000000002</v>
@@ -1774,7 +1774,7 @@
         <v>23</v>
       </c>
       <c r="C18" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D18">
         <v>399.35719999999998</v>
@@ -1844,7 +1844,7 @@
         <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D19">
         <v>552.97400000000005</v>
@@ -1914,7 +1914,7 @@
         <v>24</v>
       </c>
       <c r="C20" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D20">
         <v>1988.4891</v>
@@ -1984,7 +1984,7 @@
         <v>24</v>
       </c>
       <c r="C21" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D21">
         <v>805.03399999999999</v>
@@ -2054,7 +2054,7 @@
         <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D22">
         <v>1516.8369</v>
@@ -2124,7 +2124,7 @@
         <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D23">
         <v>517.91650000000004</v>
@@ -2194,7 +2194,7 @@
         <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D24">
         <v>467.94540000000001</v>
@@ -2264,7 +2264,7 @@
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D25">
         <v>473.34660000000002</v>
@@ -2334,7 +2334,7 @@
         <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D26">
         <v>1066.4603999999999</v>
@@ -2404,7 +2404,7 @@
         <v>24</v>
       </c>
       <c r="C27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D27">
         <v>465.16379999999998</v>
@@ -2474,7 +2474,7 @@
         <v>24</v>
       </c>
       <c r="C28" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D28">
         <v>633.58150000000001</v>
@@ -2544,7 +2544,7 @@
         <v>25</v>
       </c>
       <c r="C29" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D29">
         <v>2260.9364999999998</v>
@@ -2614,7 +2614,7 @@
         <v>25</v>
       </c>
       <c r="C30" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D30">
         <v>906.16790000000003</v>
@@ -2684,7 +2684,7 @@
         <v>25</v>
       </c>
       <c r="C31" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D31">
         <v>1727.3032000000001</v>
@@ -2754,7 +2754,7 @@
         <v>25</v>
       </c>
       <c r="C32" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D32">
         <v>599.57119999999998</v>
@@ -2824,7 +2824,7 @@
         <v>25</v>
       </c>
       <c r="C33" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D33">
         <v>548.60919999999999</v>
@@ -2894,7 +2894,7 @@
         <v>25</v>
       </c>
       <c r="C34" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D34">
         <v>554.21400000000006</v>
@@ -2964,7 +2964,7 @@
         <v>25</v>
       </c>
       <c r="C35" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D35">
         <v>1277.6552999999999</v>
@@ -3034,7 +3034,7 @@
         <v>25</v>
       </c>
       <c r="C36" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D36">
         <v>545.50720000000001</v>
@@ -3104,7 +3104,7 @@
         <v>25</v>
       </c>
       <c r="C37" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D37">
         <v>749.78589999999997</v>
@@ -3174,7 +3174,7 @@
         <v>22</v>
       </c>
       <c r="C38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D38">
         <v>3838.1801</v>
@@ -3244,7 +3244,7 @@
         <v>22</v>
       </c>
       <c r="C39" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D39">
         <v>1414.6353999999999</v>
@@ -3314,7 +3314,7 @@
         <v>22</v>
       </c>
       <c r="C40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D40">
         <v>2783.5153</v>
@@ -3384,7 +3384,7 @@
         <v>22</v>
       </c>
       <c r="C41" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D41">
         <v>823.60310000000004</v>
@@ -3454,7 +3454,7 @@
         <v>22</v>
       </c>
       <c r="C42" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D42">
         <v>787.52650000000006</v>
@@ -3524,7 +3524,7 @@
         <v>22</v>
       </c>
       <c r="C43" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D43">
         <v>790.45280000000002</v>
@@ -3594,7 +3594,7 @@
         <v>22</v>
       </c>
       <c r="C44" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D44">
         <v>1651.6928</v>
@@ -3664,7 +3664,7 @@
         <v>22</v>
       </c>
       <c r="C45" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D45">
         <v>788.12850000000003</v>
@@ -3734,7 +3734,7 @@
         <v>22</v>
       </c>
       <c r="C46" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D46">
         <v>1038.6316999999999</v>
@@ -3804,7 +3804,7 @@
         <v>23</v>
       </c>
       <c r="C47" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D47">
         <v>1667.9771000000001</v>
@@ -3874,7 +3874,7 @@
         <v>23</v>
       </c>
       <c r="C48" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D48">
         <v>661.21640000000002</v>
@@ -3944,7 +3944,7 @@
         <v>23</v>
       </c>
       <c r="C49" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D49">
         <v>1249.7942</v>
@@ -4014,7 +4014,7 @@
         <v>23</v>
       </c>
       <c r="C50" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D50">
         <v>454.9683</v>
@@ -4084,7 +4084,7 @@
         <v>23</v>
       </c>
       <c r="C51" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D51">
         <v>402.68029999999999</v>
@@ -4154,7 +4154,7 @@
         <v>23</v>
       </c>
       <c r="C52" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D52">
         <v>408.50029999999998</v>
@@ -4224,7 +4224,7 @@
         <v>23</v>
       </c>
       <c r="C53" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D53">
         <v>963.07600000000002</v>
@@ -4294,7 +4294,7 @@
         <v>23</v>
       </c>
       <c r="C54" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D54">
         <v>399.35719999999998</v>
@@ -4364,7 +4364,7 @@
         <v>23</v>
       </c>
       <c r="C55" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D55">
         <v>552.97400000000005</v>
@@ -4434,7 +4434,7 @@
         <v>24</v>
       </c>
       <c r="C56" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D56">
         <v>1988.4891</v>
@@ -4504,7 +4504,7 @@
         <v>24</v>
       </c>
       <c r="C57" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D57">
         <v>805.03399999999999</v>
@@ -4574,7 +4574,7 @@
         <v>24</v>
       </c>
       <c r="C58" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D58">
         <v>1516.8369</v>
@@ -4644,7 +4644,7 @@
         <v>24</v>
       </c>
       <c r="C59" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D59">
         <v>517.91650000000004</v>
@@ -4714,7 +4714,7 @@
         <v>24</v>
       </c>
       <c r="C60" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D60">
         <v>467.94540000000001</v>
@@ -4784,7 +4784,7 @@
         <v>24</v>
       </c>
       <c r="C61" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D61">
         <v>473.34660000000002</v>
@@ -4854,7 +4854,7 @@
         <v>24</v>
       </c>
       <c r="C62" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D62">
         <v>1066.4603999999999</v>
@@ -4924,7 +4924,7 @@
         <v>24</v>
       </c>
       <c r="C63" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D63">
         <v>465.16379999999998</v>
@@ -4994,7 +4994,7 @@
         <v>24</v>
       </c>
       <c r="C64" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D64">
         <v>633.58150000000001</v>
@@ -5064,7 +5064,7 @@
         <v>25</v>
       </c>
       <c r="C65" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D65">
         <v>2260.9364999999998</v>
@@ -5134,7 +5134,7 @@
         <v>25</v>
       </c>
       <c r="C66" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D66">
         <v>906.16790000000003</v>
@@ -5204,7 +5204,7 @@
         <v>25</v>
       </c>
       <c r="C67" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D67">
         <v>1727.3032000000001</v>
@@ -5274,7 +5274,7 @@
         <v>25</v>
       </c>
       <c r="C68" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D68">
         <v>599.57119999999998</v>
@@ -5344,7 +5344,7 @@
         <v>25</v>
       </c>
       <c r="C69" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D69">
         <v>548.60919999999999</v>
@@ -5414,7 +5414,7 @@
         <v>25</v>
       </c>
       <c r="C70" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D70">
         <v>554.21400000000006</v>
@@ -5484,7 +5484,7 @@
         <v>25</v>
       </c>
       <c r="C71" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D71">
         <v>1277.6552999999999</v>
@@ -5554,7 +5554,7 @@
         <v>25</v>
       </c>
       <c r="C72" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D72">
         <v>545.50720000000001</v>
@@ -5624,7 +5624,7 @@
         <v>25</v>
       </c>
       <c r="C73" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D73">
         <v>749.78589999999997</v>
@@ -5687,7 +5687,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:V1" xr:uid="{C0070676-F8E8-4A46-A33E-42545481B390}"/>
+  <autoFilter ref="A1:V73" xr:uid="{C0070676-F8E8-4A46-A33E-42545481B390}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>